<commit_message>
updated requiremewnt document for registration client.
</commit_message>
<xml_diff>
--- a/requirements/MOSIP_Requirements Change_Tracker_27Nov18.xlsx
+++ b/requirements/MOSIP_Requirements Change_Tracker_27Nov18.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\Desktop\PROJECTS\MOSIP\Bootcamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1047454\git\mosip_master\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A4390250-1AB9-463D-9E64-903C167966F6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="462"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_QueryLog_External" sheetId="5" r:id="rId1"/>
@@ -18,9 +17,9 @@
     <sheet name="Pivot" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_QueryLog_External!$A$2:$Q$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_QueryLog_External!$A$2:$Q$67</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="217">
   <si>
     <t>MOSIP - Requirements Change Log</t>
   </si>
@@ -2520,11 +2519,28 @@
   <si>
     <t>Shrikant/Ramesh</t>
   </si>
+  <si>
+    <t xml:space="preserve">Statsus Updated to Exported for the exported.
+FilePath should be a configurable one.
+Offline only export should work.
+Serice changes, UI changes. 
+EOD Approval Screen On/Off. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Pre-Reg Sync/Batch Job Changes
+2. Multi-lingual changes 
+3. ID object based strucutre changes </t>
+  </si>
+  <si>
+    <t>1. UI change.
+2. Service and Dao changes.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -2969,7 +2985,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2986,7 +3002,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:Q56" sheet="MOSIP_QueryLog_External"/>
   </cacheSource>
@@ -4147,7 +4163,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -4495,37 +4511,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q63" sqref="Q63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.26953125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="71.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="20" customWidth="1"/>
-    <col min="8" max="8" width="44.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="46" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="71.1796875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="44.453125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" style="46" customWidth="1"/>
+    <col min="14" max="14" width="15.81640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="24.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.81640625" style="2" customWidth="1"/>
     <col min="17" max="17" width="35" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="20.28515625" style="12"/>
+    <col min="18" max="16384" width="20.26953125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -4546,7 +4563,7 @@
       <c r="P1" s="67"/>
       <c r="Q1" s="69"/>
     </row>
-    <row r="2" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
@@ -4599,7 +4616,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4648,7 +4665,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -4697,7 +4714,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -4746,7 +4763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -4795,7 +4812,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -4843,7 +4860,7 @@
       <c r="P7" s="36"/>
       <c r="Q7" s="26"/>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" s="1" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -4890,7 +4907,7 @@
       <c r="P8" s="36"/>
       <c r="Q8" s="26"/>
     </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" ht="213.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -4937,7 +4954,7 @@
       <c r="P9" s="36"/>
       <c r="Q9" s="26"/>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" s="1" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -4986,7 +5003,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" ht="98.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" s="1" customFormat="1" ht="98.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -5039,7 +5056,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" s="1" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -5092,7 +5109,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -5145,7 +5162,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -5198,7 +5215,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="60" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="60" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -5251,7 +5268,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -5304,7 +5321,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -5357,7 +5374,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="252" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -5408,7 +5425,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -5461,7 +5478,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -5514,7 +5531,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -5563,7 +5580,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="63" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="63" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -5614,7 +5631,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -5667,7 +5684,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -5714,7 +5731,7 @@
       <c r="P24" s="36"/>
       <c r="Q24" s="18"/>
     </row>
-    <row r="25" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -5755,7 +5772,7 @@
       <c r="P25" s="36"/>
       <c r="Q25" s="38"/>
     </row>
-    <row r="26" spans="1:17" s="10" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" s="10" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -5804,7 +5821,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="10" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="10" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -5853,7 +5870,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -5900,7 +5917,7 @@
       <c r="P28" s="36"/>
       <c r="Q28" s="18"/>
     </row>
-    <row r="29" spans="1:17" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -5950,7 +5967,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -5999,7 +6016,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -6044,7 +6061,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -6089,7 +6106,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -6132,7 +6149,7 @@
       <c r="P33" s="36"/>
       <c r="Q33" s="38"/>
     </row>
-    <row r="34" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -6175,7 +6192,7 @@
       <c r="P34" s="36"/>
       <c r="Q34" s="38"/>
     </row>
-    <row r="35" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -6218,7 +6235,7 @@
       <c r="P35" s="36"/>
       <c r="Q35" s="38"/>
     </row>
-    <row r="36" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -6261,7 +6278,7 @@
       <c r="P36" s="36"/>
       <c r="Q36" s="38"/>
     </row>
-    <row r="37" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -6310,7 +6327,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -6355,7 +6372,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -6398,7 +6415,7 @@
       <c r="P39" s="36"/>
       <c r="Q39" s="38"/>
     </row>
-    <row r="40" spans="1:17" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -6441,7 +6458,7 @@
       <c r="P40" s="36"/>
       <c r="Q40" s="38"/>
     </row>
-    <row r="41" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -6490,7 +6507,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -6533,7 +6550,7 @@
       <c r="P42" s="36"/>
       <c r="Q42" s="38"/>
     </row>
-    <row r="43" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -6576,7 +6593,7 @@
       <c r="P43" s="36"/>
       <c r="Q43" s="38"/>
     </row>
-    <row r="44" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -6625,7 +6642,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -6674,7 +6691,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -6717,7 +6734,7 @@
       <c r="P46" s="36"/>
       <c r="Q46" s="38"/>
     </row>
-    <row r="47" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -6760,7 +6777,7 @@
       <c r="P47" s="36"/>
       <c r="Q47" s="38"/>
     </row>
-    <row r="48" spans="1:17" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -6809,7 +6826,7 @@
       <c r="P48" s="36"/>
       <c r="Q48" s="38"/>
     </row>
-    <row r="49" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>47</v>
       </c>
@@ -6854,7 +6871,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -6897,7 +6914,7 @@
       <c r="P50" s="39"/>
       <c r="Q50" s="38"/>
     </row>
-    <row r="51" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>49</v>
       </c>
@@ -6940,7 +6957,7 @@
       <c r="P51" s="39"/>
       <c r="Q51" s="38"/>
     </row>
-    <row r="52" spans="1:17" ht="171" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -6989,7 +7006,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -7038,7 +7055,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -7081,7 +7098,7 @@
       <c r="P54" s="39"/>
       <c r="Q54" s="38"/>
     </row>
-    <row r="55" spans="1:17" ht="228" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" ht="210" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -7118,13 +7135,19 @@
       <c r="L55" s="26">
         <v>43446</v>
       </c>
-      <c r="M55" s="37"/>
-      <c r="N55" s="5"/>
+      <c r="M55" s="37">
+        <v>12</v>
+      </c>
+      <c r="N55" s="5">
+        <v>24</v>
+      </c>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
-      <c r="Q55" s="38"/>
-    </row>
-    <row r="56" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="Q55" s="38" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="42" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -7161,13 +7184,17 @@
       <c r="L56" s="26">
         <v>43446</v>
       </c>
-      <c r="M56" s="37"/>
-      <c r="N56" s="5"/>
+      <c r="M56" s="37">
+        <v>2</v>
+      </c>
+      <c r="N56" s="5">
+        <v>4</v>
+      </c>
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
       <c r="Q56" s="38"/>
     </row>
-    <row r="57" spans="1:17" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -7204,13 +7231,19 @@
       <c r="L57" s="26">
         <v>43451</v>
       </c>
-      <c r="M57" s="37"/>
-      <c r="N57" s="5"/>
+      <c r="M57" s="37">
+        <v>9</v>
+      </c>
+      <c r="N57" s="5">
+        <v>18</v>
+      </c>
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
-      <c r="Q57" s="38"/>
-    </row>
-    <row r="58" spans="1:17" ht="114" x14ac:dyDescent="0.25">
+      <c r="Q57" s="38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -7253,7 +7286,7 @@
       <c r="P58" s="5"/>
       <c r="Q58" s="38"/>
     </row>
-    <row r="59" spans="1:17" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" ht="112" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -7290,13 +7323,19 @@
       <c r="L59" s="52">
         <v>43452</v>
       </c>
-      <c r="M59" s="53"/>
-      <c r="N59" s="54"/>
+      <c r="M59" s="53">
+        <v>8</v>
+      </c>
+      <c r="N59" s="54">
+        <v>16</v>
+      </c>
       <c r="O59" s="54"/>
       <c r="P59" s="54"/>
-      <c r="Q59" s="34"/>
-    </row>
-    <row r="60" spans="1:17" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="Q59" s="34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -7339,7 +7378,7 @@
       <c r="P60" s="5"/>
       <c r="Q60" s="38"/>
     </row>
-    <row r="61" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -7390,7 +7429,7 @@
       </c>
       <c r="Q61" s="34"/>
     </row>
-    <row r="62" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -7441,7 +7480,7 @@
       </c>
       <c r="Q62" s="38"/>
     </row>
-    <row r="63" spans="1:17" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" ht="126" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -7484,7 +7523,7 @@
       <c r="P63" s="5"/>
       <c r="Q63" s="38"/>
     </row>
-    <row r="64" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" ht="84" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -7527,7 +7566,7 @@
       <c r="P64" s="5"/>
       <c r="Q64" s="38"/>
     </row>
-    <row r="65" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" ht="56" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -7570,7 +7609,7 @@
       <c r="P65" s="5"/>
       <c r="Q65" s="38"/>
     </row>
-    <row r="66" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" ht="56" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -7613,7 +7652,7 @@
       <c r="P66" s="5"/>
       <c r="Q66" s="38"/>
     </row>
-    <row r="67" spans="1:17" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" ht="140" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -7656,7 +7695,7 @@
       <c r="P67" s="5"/>
       <c r="Q67" s="38"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -7676,7 +7715,23 @@
       <c r="Q68" s="38"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Q62" xr:uid="{134872B1-5513-4DED-8302-378650E5FFBD}"/>
+  <autoFilter ref="A2:Q67">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Registration Client"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="New"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="13">
+      <filters blank="1">
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:Q1"/>
   </mergeCells>
@@ -7686,57 +7741,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B11" s="11"/>
     </row>
   </sheetData>
@@ -7746,19 +7801,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>154</v>
       </c>
@@ -7769,7 +7824,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>66</v>
       </c>
@@ -7780,7 +7835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="41" t="s">
         <v>39</v>
       </c>
@@ -7791,7 +7846,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="41" t="s">
         <v>128</v>
       </c>
@@ -7802,7 +7857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="41" t="s">
         <v>74</v>
       </c>
@@ -7813,7 +7868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="41" t="s">
         <v>16</v>
       </c>
@@ -7824,7 +7879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="41" t="s">
         <v>48</v>
       </c>
@@ -7835,7 +7890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="41" t="s">
         <v>58</v>
       </c>
@@ -7846,7 +7901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="41" t="s">
         <v>155</v>
       </c>
@@ -7864,15 +7919,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8044,6 +8090,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -8068,14 +8123,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8089,6 +8136,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated CR estimates for IDA
</commit_message>
<xml_diff>
--- a/requirements/MOSIP_Requirements Change_Tracker_27Nov18.xlsx
+++ b/requirements/MOSIP_Requirements Change_Tracker_27Nov18.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1047454\git\mosip_master\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mindtree\Projects\MOSIP\IDA\Code\git-repo\master-branch\mosip\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="218">
   <si>
     <t>MOSIP - Requirements Change Log</t>
   </si>
@@ -2535,6 +2535,9 @@
   <si>
     <t>1. UI change.
 2. Service and Dao changes.</t>
+  </si>
+  <si>
+    <t>Currently, we have implemented exact, partial and phonetics. We will disable partial and phonetics for demo auth and add configuration for exact match only.</t>
   </si>
 </sst>
 </file>
@@ -4163,7 +4166,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -4515,9 +4518,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q63" sqref="Q63"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.26953125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -4812,7 +4815,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -5917,7 +5920,7 @@
       <c r="P28" s="36"/>
       <c r="Q28" s="18"/>
     </row>
-    <row r="29" spans="1:17" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="126" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -6016,7 +6019,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="140" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -6053,15 +6056,17 @@
       <c r="L31" s="26">
         <v>43440</v>
       </c>
-      <c r="M31" s="37"/>
+      <c r="M31" s="37">
+        <v>10</v>
+      </c>
       <c r="N31" s="36"/>
       <c r="O31" s="36"/>
       <c r="P31" s="36"/>
       <c r="Q31" s="38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="70" hidden="1" x14ac:dyDescent="0.35">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="70" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -6098,7 +6103,9 @@
       <c r="L32" s="26">
         <v>43440</v>
       </c>
-      <c r="M32" s="37"/>
+      <c r="M32" s="37">
+        <v>0</v>
+      </c>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
       <c r="P32" s="36"/>
@@ -6327,7 +6334,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" ht="56" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -6364,7 +6371,9 @@
       <c r="L38" s="26">
         <v>43440</v>
       </c>
-      <c r="M38" s="37"/>
+      <c r="M38" s="37">
+        <v>0</v>
+      </c>
       <c r="N38" s="36"/>
       <c r="O38" s="36"/>
       <c r="P38" s="36"/>
@@ -6826,7 +6835,7 @@
       <c r="P48" s="36"/>
       <c r="Q48" s="38"/>
     </row>
-    <row r="49" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" ht="42" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>47</v>
       </c>
@@ -6863,7 +6872,9 @@
       <c r="L49" s="26">
         <v>43440</v>
       </c>
-      <c r="M49" s="37"/>
+      <c r="M49" s="37">
+        <v>0</v>
+      </c>
       <c r="N49" s="36"/>
       <c r="O49" s="36"/>
       <c r="P49" s="36"/>
@@ -7098,7 +7109,7 @@
       <c r="P54" s="39"/>
       <c r="Q54" s="38"/>
     </row>
-    <row r="55" spans="1:17" ht="210" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" ht="210" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -7147,7 +7158,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="42" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -7194,7 +7205,7 @@
       <c r="P56" s="5"/>
       <c r="Q56" s="38"/>
     </row>
-    <row r="57" spans="1:17" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" ht="106.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -7286,7 +7297,7 @@
       <c r="P58" s="5"/>
       <c r="Q58" s="38"/>
     </row>
-    <row r="59" spans="1:17" ht="112" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -7480,7 +7491,7 @@
       </c>
       <c r="Q62" s="38"/>
     </row>
-    <row r="63" spans="1:17" ht="126" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -7523,7 +7534,7 @@
       <c r="P63" s="5"/>
       <c r="Q63" s="38"/>
     </row>
-    <row r="64" spans="1:17" ht="84" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -7566,7 +7577,7 @@
       <c r="P64" s="5"/>
       <c r="Q64" s="38"/>
     </row>
-    <row r="65" spans="1:17" ht="56" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -7609,7 +7620,7 @@
       <c r="P65" s="5"/>
       <c r="Q65" s="38"/>
     </row>
-    <row r="66" spans="1:17" ht="56" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -7652,7 +7663,7 @@
       <c r="P66" s="5"/>
       <c r="Q66" s="38"/>
     </row>
-    <row r="67" spans="1:17" ht="140" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -7718,7 +7729,7 @@
   <autoFilter ref="A2:Q67">
     <filterColumn colId="3">
       <filters>
-        <filter val="Registration Client"/>
+        <filter val="ID Authentication"/>
       </filters>
     </filterColumn>
     <filterColumn colId="4">
@@ -7919,6 +7930,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8090,39 +8133,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8138,28 +8173,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>